<commit_message>
Updated Sequence Diagrams, Update Review sheets , Update Scope Statment, Update Project Charter, Update Project Schedule, Update Scope Managment Plan
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA2D00E-4E59-4FFC-9D8D-80535880C54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC33AAF9-7D3E-4A34-997D-E986DE709B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Comment ID</t>
   </si>
@@ -189,35 +189,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="1"/>
       <scheme val="minor"/>
     </font>
@@ -225,7 +225,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -233,7 +233,7 @@
       <b/>
       <sz val="16"/>
       <color theme="4" tint="-0.499984740745262"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -241,28 +241,28 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF002060"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -336,23 +336,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,49 +636,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="68.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="23.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.296875" customWidth="1"/>
+    <col min="4" max="4" width="20.296875" customWidth="1"/>
+    <col min="5" max="5" width="68.09765625" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="26.8984375" customWidth="1"/>
+    <col min="8" max="8" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
@@ -691,20 +691,20 @@
       <c r="D2" s="11">
         <v>44685</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="17">
         <v>44747</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -717,20 +717,20 @@
       <c r="D3" s="11">
         <v>44685</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="17">
         <v>44747</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -743,16 +743,16 @@
       <c r="D4" s="11">
         <v>44685</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -765,16 +765,16 @@
       <c r="D5" s="11">
         <v>44685</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-    </row>
-    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -787,16 +787,18 @@
       <c r="D6" s="11">
         <v>44685</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -809,16 +811,18 @@
       <c r="D7" s="12">
         <v>44685</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-    </row>
-    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -831,16 +835,16 @@
       <c r="D8" s="12">
         <v>44685</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -853,16 +857,18 @@
       <c r="D9" s="11">
         <v>44685</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -875,20 +881,20 @@
       <c r="D10" s="11">
         <v>44685</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="17">
         <v>44747</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
@@ -901,20 +907,20 @@
       <c r="D11" s="11">
         <v>44685</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="17">
         <v>44717</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
@@ -927,20 +933,20 @@
       <c r="D12" s="11">
         <v>44685</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="17">
         <v>44747</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
@@ -953,16 +959,16 @@
       <c r="D13" s="11">
         <v>44685</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>37</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
@@ -975,16 +981,16 @@
       <c r="D14" s="11">
         <v>44685</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="14" t="s">
         <v>38</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
@@ -997,23 +1003,23 @@
       <c r="D15" s="11">
         <v>44685</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
@@ -1099,14 +1105,14 @@
       <c r="D28" s="7"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="8"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1120,14 +1126,14 @@
       <c r="D31" s="7"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="8"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>

</xml_diff>

<commit_message>
Updated Sequence Diagrams, Remove Feedback from SRS, Sequence Digarm
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC33AAF9-7D3E-4A34-997D-E986DE709B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF0B7F5-55C2-4C87-B0C1-5A87E92F3926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Sequence Diagrams, Comments on wireframe in Reviews, Updated ERD
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF0B7F5-55C2-4C87-B0C1-5A87E92F3926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62533AF-70AC-4F41-9DBC-F25B3B010A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>Comment ID</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>PMP/Issue management</t>
+  </si>
+  <si>
+    <t>Osama</t>
+  </si>
+  <si>
+    <t>Medhat</t>
   </si>
 </sst>
 </file>
@@ -746,10 +752,12 @@
       <c r="E4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="16"/>
+      <c r="F4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>51</v>
+      </c>
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
@@ -838,10 +846,12 @@
       <c r="E8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="16"/>
+      <c r="F8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
@@ -962,10 +972,12 @@
       <c r="E13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="16"/>
+      <c r="F13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
@@ -984,10 +996,12 @@
       <c r="E14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="16"/>
+      <c r="F14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding low level flowcharts
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC33AAF9-7D3E-4A34-997D-E986DE709B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62533AF-70AC-4F41-9DBC-F25B3B010A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>Comment ID</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>PMP/Issue management</t>
+  </si>
+  <si>
+    <t>Osama</t>
+  </si>
+  <si>
+    <t>Medhat</t>
   </si>
 </sst>
 </file>
@@ -637,7 +643,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -746,10 +752,12 @@
       <c r="E4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="16"/>
+      <c r="F4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>51</v>
+      </c>
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
@@ -838,10 +846,12 @@
       <c r="E8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="16"/>
+      <c r="F8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
@@ -962,10 +972,12 @@
       <c r="E13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="16"/>
+      <c r="F13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
@@ -984,10 +996,12 @@
       <c r="E14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="16"/>
+      <c r="F14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating PMP and Issue managment
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587287B-6CA1-4A6F-8790-13DAC4E80D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7E7177-E119-4C3F-9FB6-2A89EB496773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Comment ID</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>LLD is missing</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>CM</t>
@@ -194,7 +191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,13 +252,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
@@ -308,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -330,19 +320,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -646,7 +633,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H6" sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,387 +649,389 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="16">
+        <v>44747</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="16">
+        <v>44747</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="16">
+        <v>44839</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="11">
+        <v>44685</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="11">
+        <v>44685</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="16">
+        <v>44747</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="H11" s="16">
+        <v>44717</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="16">
+        <v>44747</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="10">
+        <v>44685</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="17">
-        <v>44747</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="17">
-        <v>44747</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="12">
-        <v>44685</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="12">
-        <v>44685</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="17">
-        <v>44747</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="17">
-        <v>44717</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="17">
-        <v>44747</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="11">
-        <v>44685</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="17">
+      <c r="H15" s="16">
         <v>44839</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>

</xml_diff>

<commit_message>
updating SRS,PMP,Audits,layout and RTM
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7E7177-E119-4C3F-9FB6-2A89EB496773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5E134-047C-4C47-B49D-1A44D6689AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <t>Comment ID</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Ashry</t>
+  </si>
+  <si>
+    <t>13/5/2022</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:H15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,7 +751,9 @@
       <c r="G4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="16">
+        <v>44809</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -798,7 +803,9 @@
       <c r="G6" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="16">
+        <v>44839</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -822,7 +829,9 @@
       <c r="G7" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="16">
+        <v>44839</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -846,7 +855,9 @@
       <c r="G8" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="15"/>
+      <c r="H8" s="16">
+        <v>44839</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -870,7 +881,9 @@
       <c r="G9" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="15"/>
+      <c r="H9" s="16">
+        <v>44839</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -972,7 +985,9 @@
       <c r="G13" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -996,7 +1011,9 @@
       <c r="G14" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="15"/>
+      <c r="H14" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">

</xml_diff>

<commit_message>
Adding comments from the previous audit.
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5E134-047C-4C47-B49D-1A44D6689AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2305E7-9F21-4CF1-AD18-7C05C7141884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Comment ID</t>
   </si>
@@ -188,6 +196,30 @@
   </si>
   <si>
     <t>13/5/2022</t>
+  </si>
+  <si>
+    <t>Auditer\ Mohamed Hassan</t>
+  </si>
+  <si>
+    <t>15/5/20222</t>
+  </si>
+  <si>
+    <t>17/5/2022</t>
+  </si>
+  <si>
+    <t>The message in the login sequence diagram need to be the same message as the same as the message written in the SRS and in the code in the system.</t>
+  </si>
+  <si>
+    <t>15/5/2022</t>
+  </si>
+  <si>
+    <t>The sequence diagram should be added to the high-level design and removed from LLD.</t>
+  </si>
+  <si>
+    <t>Impact analysis</t>
+  </si>
+  <si>
+    <t>Impact analysis should be re-written again.</t>
   </si>
 </sst>
 </file>
@@ -198,35 +230,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="1"/>
       <scheme val="minor"/>
     </font>
@@ -234,7 +266,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -242,7 +274,7 @@
       <b/>
       <sz val="16"/>
       <color theme="4" tint="-0.499984740745262"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -250,21 +282,21 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF002060"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -301,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -352,6 +384,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,23 +673,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="68.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="2" width="23.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.296875" customWidth="1"/>
+    <col min="4" max="4" width="20.296875" customWidth="1"/>
+    <col min="5" max="5" width="68.09765625" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="26.8984375" customWidth="1"/>
+    <col min="8" max="8" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -677,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -703,7 +741,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -729,7 +767,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -755,7 +793,7 @@
         <v>44809</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -781,7 +819,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -807,7 +845,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
@@ -833,7 +871,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -859,7 +897,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -885,7 +923,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
@@ -911,7 +949,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
@@ -937,7 +975,7 @@
         <v>44717</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
@@ -963,7 +1001,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
@@ -989,7 +1027,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>20</v>
       </c>
@@ -1015,7 +1053,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1079,7 @@
         <v>44839</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1050,119 +1088,176 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="7"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="7"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="8"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="8"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="7"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="8"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>

</xml_diff>

<commit_message>
Create Test Plan,Update excecution of test cases, Create Bug Report, Update Audit sheet
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\Travel_Advisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2305E7-9F21-4CF1-AD18-7C05C7141884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD4B0C6-3918-4017-A9CA-BFD8A43989A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>Comment ID</t>
   </si>
@@ -220,13 +220,49 @@
   </si>
   <si>
     <t>Impact analysis should be re-written again.</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>22/5/20222</t>
+  </si>
+  <si>
+    <t>The test cases data steps is unclear enough.</t>
+  </si>
+  <si>
+    <t>25/5/2022</t>
+  </si>
+  <si>
+    <t>24/5/2022</t>
+  </si>
+  <si>
+    <t>Auditer\Mohamed Hassan</t>
+  </si>
+  <si>
+    <t>The test case in user book is unclear in precondition.</t>
+  </si>
+  <si>
+    <t>RTM must be reviewed against SRS.</t>
+  </si>
+  <si>
+    <t>All Team</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>RTM</t>
+  </si>
+  <si>
+    <t>The test case in user book is missing REQ-03-Tour.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,13 +290,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="1"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -333,11 +362,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -349,10 +375,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -361,10 +387,10 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -379,17 +405,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -690,424 +716,424 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="C2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="9">
         <v>44685</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="15">
         <v>44747</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="9">
         <v>44685</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>44747</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="9">
         <v>44685</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="F4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>44809</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="9">
         <v>44685</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="15" t="s">
+      <c r="F5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <v>44839</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9">
         <v>44685</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>44839</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="10">
         <v>44685</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="F7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <v>44839</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="10">
         <v>44685</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="15" t="s">
+      <c r="F8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <v>44839</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="9">
         <v>44685</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="15" t="s">
+      <c r="F9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <v>44839</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="C10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="9">
         <v>44685</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="15" t="s">
+      <c r="F10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>44747</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="9">
         <v>44685</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="15" t="s">
+      <c r="F11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <v>44717</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9">
         <v>44685</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <v>44747</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="9">
         <v>44685</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="9">
         <v>44685</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="10">
+      <c r="C15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="9">
         <v>44685</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="15" t="s">
+      <c r="F15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <v>44839</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="20" t="s">
+      <c r="F17" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>47</v>
       </c>
       <c r="H17" t="s">
@@ -1115,25 +1141,25 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="20" t="s">
+      <c r="F18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>47</v>
       </c>
       <c r="H18" t="s">
@@ -1141,139 +1167,222 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="20" t="s">
+      <c r="F19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>47</v>
       </c>
       <c r="H19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="3"/>
+    <row r="20" spans="1:8" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="3"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="2"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="7"/>
       <c r="E34" s="3"/>
     </row>
+    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Test case execution, Update RTM , Update Bug report, Create Test excution Summary, Bug report Summary,Update Impact Analysis, Update Reviews sheet
</commit_message>
<xml_diff>
--- a/Audits.xlsx
+++ b/Audits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\Travel_Advisor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD4B0C6-3918-4017-A9CA-BFD8A43989A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE15F24-90AE-4689-8F0D-77D075425D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="74">
   <si>
     <t>Comment ID</t>
   </si>
@@ -249,13 +249,13 @@
     <t>All Team</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>RTM</t>
   </si>
   <si>
     <t>The test case in user book is missing REQ-03-Tour.</t>
+  </si>
+  <si>
+    <t>22/5/2022</t>
   </si>
 </sst>
 </file>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1267,7 @@
         <v>63</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>44</v>
@@ -1284,22 +1284,25 @@
         <v>11</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>69</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>